<commit_message>
Added 1st and 2nd task
</commit_message>
<xml_diff>
--- a/MREZA_CESTOVNIH_PRAVACA.xlsx
+++ b/MREZA_CESTOVNIH_PRAVACA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E224185B-4D0E-4039-B0BA-AB276FD92C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE415306-A697-4536-9AA4-52B19F9F7681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MREŽA CESTOVNIH PRAVACA" sheetId="3" r:id="rId1"/>
@@ -213,12 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A7DD6A-5C38-4119-AE6E-7E25FE5531AA}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,10 +1159,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1181,10 +1180,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1202,10 +1201,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1223,19 +1222,19 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="1">
         <v>53.5</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="1">
         <v>55.1</v>
       </c>
       <c r="F36" s="3">
@@ -1244,19 +1243,19 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="1">
         <v>50.5</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="1">
         <v>52.3</v>
       </c>
       <c r="F37" s="3">
@@ -1265,19 +1264,19 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="1">
         <v>70.3</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="1">
         <v>98.2</v>
       </c>
       <c r="F38" s="3">
@@ -1286,19 +1285,19 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="1">
         <v>206</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="1">
         <v>114.4</v>
       </c>
       <c r="F39" s="3">
@@ -1307,19 +1306,19 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="1">
         <v>51.6</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="1">
         <v>68.2</v>
       </c>
       <c r="F40" s="3">
@@ -1328,45 +1327,45 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="4">
-        <v>378</v>
-      </c>
-      <c r="E41" s="4">
-        <v>109.2</v>
+      <c r="A41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="1">
+        <v>52.8</v>
+      </c>
+      <c r="E41" s="1">
+        <v>75.2</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="0"/>
-        <v>207.69230769230768</v>
+        <v>42.127659574468076</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="4">
-        <v>442</v>
-      </c>
-      <c r="E42" s="4">
-        <v>110.5</v>
+      <c r="C42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="1">
+        <v>89.7</v>
+      </c>
+      <c r="E42" s="1">
+        <v>60.3</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="0"/>
-        <v>240</v>
+        <v>89.25373134328359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>